<commit_message>
Sincos unit validation complete. Timing closure next.
</commit_message>
<xml_diff>
--- a/doc/design/sincos_error.xlsx
+++ b/doc/design/sincos_error.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="22960" tabRatio="500" activeTab="4"/>
@@ -1462,11 +1462,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2131486360"/>
-        <c:axId val="2131489384"/>
+        <c:axId val="2124380200"/>
+        <c:axId val="2125302152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2131486360"/>
+        <c:axId val="2124380200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1476,7 +1476,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2131489384"/>
+        <c:crossAx val="2125302152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1484,7 +1484,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2131489384"/>
+        <c:axId val="2125302152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1495,7 +1495,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2131486360"/>
+        <c:crossAx val="2124380200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -59442,7 +59442,7 @@
   <dimension ref="A1:W79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:XFD22"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -59540,6 +59540,17 @@
         <f t="shared" si="0"/>
         <v>402</v>
       </c>
+      <c r="E9">
+        <v>-2.0511240000000002</v>
+      </c>
+      <c r="F9">
+        <f>SIN(E9)</f>
+        <v>-0.88684356250129026</v>
+      </c>
+      <c r="G9">
+        <f>COS(E9)</f>
+        <v>-0.46206979521498714</v>
+      </c>
     </row>
     <row r="10" spans="1:23">
       <c r="A10">

</xml_diff>

<commit_message>
Added draft of the t_block hardware design.
</commit_message>
<xml_diff>
--- a/doc/design/sincos_error.xlsx
+++ b/doc/design/sincos_error.xlsx
@@ -1462,11 +1462,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2124380200"/>
-        <c:axId val="2125302152"/>
+        <c:axId val="2087849944"/>
+        <c:axId val="2087846952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2124380200"/>
+        <c:axId val="2087849944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1476,7 +1476,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2125302152"/>
+        <c:crossAx val="2087846952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1484,7 +1484,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2125302152"/>
+        <c:axId val="2087846952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1495,7 +1495,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2124380200"/>
+        <c:crossAx val="2087849944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -59442,7 +59442,7 @@
   <dimension ref="A1:W79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E9" sqref="E9:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -59540,17 +59540,6 @@
         <f t="shared" si="0"/>
         <v>402</v>
       </c>
-      <c r="E9">
-        <v>-2.0511240000000002</v>
-      </c>
-      <c r="F9">
-        <f>SIN(E9)</f>
-        <v>-0.88684356250129026</v>
-      </c>
-      <c r="G9">
-        <f>COS(E9)</f>
-        <v>-0.46206979521498714</v>
-      </c>
     </row>
     <row r="10" spans="1:23">
       <c r="A10">

</xml_diff>

<commit_message>
Adding a whole other hardware directory for a shrunk version of ik_swift, ik_swift_32. Finding bitwidths to shrink while preserving convergence.
</commit_message>
<xml_diff>
--- a/doc/design/sincos_error.xlsx
+++ b/doc/design/sincos_error.xlsx
@@ -1498,11 +1498,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2142849320"/>
-        <c:axId val="2142852344"/>
+        <c:axId val="-2126128696"/>
+        <c:axId val="-2129315144"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2142849320"/>
+        <c:axId val="-2126128696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1512,7 +1512,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142852344"/>
+        <c:crossAx val="-2129315144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1520,7 +1520,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2142852344"/>
+        <c:axId val="-2129315144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1531,7 +1531,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142849320"/>
+        <c:crossAx val="-2126128696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2414,11 +2414,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2142020008"/>
-        <c:axId val="2142022984"/>
+        <c:axId val="-2126072056"/>
+        <c:axId val="-2126069080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2142020008"/>
+        <c:axId val="-2126072056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2428,7 +2428,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142022984"/>
+        <c:crossAx val="-2126069080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2436,7 +2436,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2142022984"/>
+        <c:axId val="-2126069080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2447,13 +2447,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142020008"/>
+        <c:crossAx val="-2126072056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -66831,8 +66832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>